<commit_message>
Update: updated for fall-25 & spring-26 - version 1.3
</commit_message>
<xml_diff>
--- a/uploads/xlsx/Timetable SE Department (Fall-25 & Spring-26) Version-1.3-updated.xlsx
+++ b/uploads/xlsx/Timetable SE Department (Fall-25 & Spring-26) Version-1.3-updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\zPythonStuff\Superior Academic Tool\uploads\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EBF53AB-0FC2-44BA-B93E-24B281C8028D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381FB84E-8C5A-4092-BF24-9A2668C5AAD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="577" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="577" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Time Table" sheetId="1" r:id="rId1"/>
@@ -755,11 +755,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Software Re-Engineering 
-BSSE-8B
-Mr. Hammmad Ur Rehman </t>
-  </si>
-  <si>
     <t xml:space="preserve">Operations Research 
 BSSE-8B
 Mr. Hamza Hameed </t>
@@ -803,11 +798,6 @@
     <t xml:space="preserve">Natutral Language Processing 
 BSAI-8A
 Mr. Ansar Naseem </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parallel &amp; Distributed Computing 
-BSDS-7A/BSAI-7A
-Mr. Adeel </t>
   </si>
   <si>
     <r>
@@ -1023,21 +1013,6 @@
     <t xml:space="preserve">Software Quality Engineering
 BSSE-6C
 Mr. Sawail Khan </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Computer Organization &amp; Assembly Language 
-BSAI-6A
-Mr. Adeel </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Computer Organization &amp; Assembly Language 
-BSAI-6B
-Mr. Adeel </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Computer Organization &amp; Assembly Language 
-BSAI-6C/BSDS-6A
-Mr. Adeel </t>
   </si>
   <si>
     <t xml:space="preserve">Computer Organization &amp; Assembly Language (Lab)
@@ -1699,6 +1674,31 @@
     <t xml:space="preserve">Professional Practrices 
 BSSE-8D/BSAI-8A
 Mr. Umair Iftikhar </t>
+  </si>
+  <si>
+    <t>Computer Organization &amp; Assembly Language 
+BSAI-6A
+Mr. Adeel Amjad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computer Organization &amp; Assembly Language 
+BSAI-6B
+Mr. Adeel Amjad </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computer Organization &amp; Assembly Language 
+BSAI-6C/BSDS-6A
+Mr. Adeel Amjad </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parallel &amp; Distributed Computing 
+BSDS-7A/BSAI-7A
+Mr. Adeel Amjad </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Software Re-Engineering 
+BSSE-8B
+Mr. Hammad Ur Rehman </t>
   </si>
 </sst>
 </file>
@@ -5210,9 +5210,9 @@
   </sheetPr>
   <dimension ref="A1:AB1008"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F32" sqref="F32:G32"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H33" sqref="H33:I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5443,7 +5443,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="C7" s="373" t="s">
         <v>55</v>
@@ -5479,7 +5479,7 @@
     <row r="8" spans="1:28" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="337"/>
       <c r="B8" s="16" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="C8" s="374"/>
       <c r="D8" s="333" t="s">
@@ -5531,7 +5531,7 @@
         <v>92</v>
       </c>
       <c r="H9" s="194" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="I9" s="195"/>
       <c r="J9" s="250"/>
@@ -5561,15 +5561,15 @@
       </c>
       <c r="C10" s="323"/>
       <c r="D10" s="362" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E10" s="363"/>
       <c r="F10" s="364" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="G10" s="202"/>
       <c r="H10" s="192" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="I10" s="193"/>
       <c r="J10" s="127"/>
@@ -5603,7 +5603,7 @@
         <v>130</v>
       </c>
       <c r="F11" s="375" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="G11" s="376"/>
       <c r="H11" s="192" t="s">
@@ -5651,10 +5651,10 @@
         <v>69</v>
       </c>
       <c r="H12" s="87" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="I12" s="200" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="J12" s="200"/>
       <c r="K12" s="130"/>
@@ -5683,11 +5683,11 @@
       </c>
       <c r="C13" s="320"/>
       <c r="D13" s="282" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="E13" s="327"/>
       <c r="F13" s="198" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="G13" s="199"/>
       <c r="H13" s="198" t="s">
@@ -5725,11 +5725,11 @@
       </c>
       <c r="E14" s="271"/>
       <c r="F14" s="198" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="G14" s="199"/>
       <c r="H14" s="382" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I14" s="383"/>
       <c r="J14" s="220"/>
@@ -5759,7 +5759,7 @@
       </c>
       <c r="C15" s="320"/>
       <c r="D15" s="201" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="E15" s="202"/>
       <c r="G15" s="340" t="s">
@@ -5767,7 +5767,7 @@
       </c>
       <c r="H15" s="340"/>
       <c r="I15" s="189" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="J15" s="190"/>
       <c r="K15" s="109"/>
@@ -5840,7 +5840,7 @@
       </c>
       <c r="E17" s="372"/>
       <c r="F17" s="194" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="G17" s="204"/>
       <c r="H17" s="365" t="s">
@@ -5878,7 +5878,7 @@
       </c>
       <c r="E18" s="190"/>
       <c r="F18" s="192" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="G18" s="193"/>
       <c r="H18" s="192" t="s">
@@ -5886,7 +5886,7 @@
       </c>
       <c r="I18" s="193"/>
       <c r="J18" s="324" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="K18" s="216"/>
       <c r="L18" s="2"/>
@@ -5926,7 +5926,7 @@
       </c>
       <c r="I19" s="199"/>
       <c r="J19" s="192" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="K19" s="213"/>
       <c r="L19" s="2"/>
@@ -5954,15 +5954,15 @@
       </c>
       <c r="C20" s="320"/>
       <c r="D20" s="191" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E20" s="271"/>
       <c r="F20" s="214" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="G20" s="215"/>
       <c r="H20" s="192" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="I20" s="193"/>
       <c r="J20" s="133"/>
@@ -5992,11 +5992,11 @@
       </c>
       <c r="C21" s="321"/>
       <c r="D21" s="240" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="E21" s="325"/>
       <c r="F21" s="326" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="G21" s="325"/>
       <c r="H21" s="208"/>
@@ -6106,7 +6106,7 @@
     <row r="24" spans="1:28" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="378"/>
       <c r="B24" s="121" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="C24" s="373" t="s">
         <v>55</v>
@@ -6142,7 +6142,7 @@
     <row r="25" spans="1:28" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="378"/>
       <c r="B25" s="121" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="C25" s="374"/>
       <c r="D25" s="333" t="s">
@@ -6152,7 +6152,7 @@
       <c r="F25" s="334"/>
       <c r="G25" s="335"/>
       <c r="H25" s="403" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="I25" s="404"/>
       <c r="J25" s="155"/>
@@ -6194,7 +6194,7 @@
         <v>74</v>
       </c>
       <c r="H26" s="232" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="I26" s="302"/>
       <c r="J26" s="230"/>
@@ -6234,7 +6234,7 @@
         <v>58</v>
       </c>
       <c r="H27" s="389" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="I27" s="390"/>
       <c r="J27" s="214"/>
@@ -6264,15 +6264,15 @@
       </c>
       <c r="C28" s="239"/>
       <c r="D28" s="201" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="E28" s="201"/>
       <c r="F28" s="262" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="G28" s="262"/>
       <c r="H28" s="200" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="I28" s="200"/>
       <c r="J28" s="386"/>
@@ -6312,7 +6312,7 @@
       </c>
       <c r="G29" s="200"/>
       <c r="H29" s="200" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="I29" s="207"/>
       <c r="J29" s="22"/>
@@ -6350,11 +6350,11 @@
       </c>
       <c r="G30" s="193"/>
       <c r="H30" s="267" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="I30" s="391"/>
       <c r="J30" s="214" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="K30" s="216"/>
       <c r="L30" s="2"/>
@@ -6382,11 +6382,11 @@
       </c>
       <c r="C31" s="238"/>
       <c r="D31" s="193" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="E31" s="200"/>
       <c r="F31" s="349" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="G31" s="288"/>
       <c r="H31" s="22" t="s">
@@ -6422,7 +6422,7 @@
       </c>
       <c r="C32" s="238"/>
       <c r="D32" s="193" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="E32" s="200"/>
       <c r="F32" s="350" t="s">
@@ -6433,7 +6433,7 @@
         <v>124</v>
       </c>
       <c r="I32" s="296" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="J32" s="204"/>
       <c r="K32" s="114"/>
@@ -6462,19 +6462,19 @@
       </c>
       <c r="C33" s="238"/>
       <c r="D33" s="193" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="E33" s="192"/>
       <c r="F33" s="370" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G33" s="207"/>
       <c r="H33" s="200" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="I33" s="200"/>
       <c r="J33" s="193" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="K33" s="272"/>
       <c r="L33" s="2"/>
@@ -6546,11 +6546,11 @@
       </c>
       <c r="E35" s="11"/>
       <c r="F35" s="200" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="G35" s="207"/>
       <c r="H35" s="356" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="I35" s="357"/>
       <c r="J35" s="358"/>
@@ -6584,11 +6584,11 @@
       </c>
       <c r="E36" s="302"/>
       <c r="F36" s="360" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="G36" s="310"/>
       <c r="H36" s="224" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="I36" s="224"/>
       <c r="J36" s="305"/>
@@ -6620,11 +6620,11 @@
         <v>11</v>
       </c>
       <c r="D37" s="301" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="E37" s="226"/>
       <c r="F37" s="360" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="G37" s="302"/>
       <c r="H37" s="360" t="s">
@@ -6660,11 +6660,11 @@
         <v>15</v>
       </c>
       <c r="D38" s="240" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="E38" s="325"/>
       <c r="F38" s="326" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="G38" s="381"/>
       <c r="H38" s="299" t="s">
@@ -6776,7 +6776,7 @@
     <row r="41" spans="1:28" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="286"/>
       <c r="B41" s="121" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="C41" s="373" t="s">
         <v>55</v>
@@ -6812,7 +6812,7 @@
     <row r="42" spans="1:28" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="286"/>
       <c r="B42" s="121" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="C42" s="374"/>
       <c r="D42" s="333" t="s">
@@ -6858,11 +6858,11 @@
         <v>107</v>
       </c>
       <c r="F43" s="250" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="G43" s="251"/>
       <c r="H43" s="203" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="I43" s="204"/>
       <c r="J43" s="211"/>
@@ -6892,7 +6892,7 @@
       </c>
       <c r="C44" s="379"/>
       <c r="D44" s="191" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="E44" s="191"/>
       <c r="F44" s="22" t="s">
@@ -6972,11 +6972,11 @@
         <v>15</v>
       </c>
       <c r="D46" s="191" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="E46" s="191"/>
       <c r="F46" s="22" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="G46" s="99" t="s">
         <v>116</v>
@@ -6988,7 +6988,7 @@
         <v>141</v>
       </c>
       <c r="J46" s="192" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="K46" s="213"/>
       <c r="L46" s="2"/>
@@ -7016,7 +7016,7 @@
       </c>
       <c r="C47" s="379"/>
       <c r="D47" s="191" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E47" s="223"/>
       <c r="F47" s="192" t="s">
@@ -7024,7 +7024,7 @@
       </c>
       <c r="G47" s="193"/>
       <c r="H47" s="192" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I47" s="193"/>
       <c r="J47" s="120"/>
@@ -7058,11 +7058,11 @@
       </c>
       <c r="E48" s="191"/>
       <c r="F48" s="192" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="G48" s="193"/>
       <c r="H48" s="405" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="I48" s="193"/>
       <c r="J48" s="200"/>
@@ -7099,11 +7099,11 @@
         <v>123</v>
       </c>
       <c r="G49" s="200" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="H49" s="207"/>
       <c r="I49" s="397" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="J49" s="406"/>
       <c r="K49" s="109"/>
@@ -7164,11 +7164,11 @@
       </c>
       <c r="C51" s="379"/>
       <c r="D51" s="205" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="E51" s="206"/>
       <c r="F51" s="294" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="G51" s="295"/>
       <c r="I51" s="200" t="s">
@@ -7201,7 +7201,7 @@
       </c>
       <c r="C52" s="379"/>
       <c r="D52" s="339" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="E52" s="340"/>
       <c r="F52" s="248" t="s">
@@ -7247,7 +7247,7 @@
       </c>
       <c r="G53" s="207"/>
       <c r="H53" s="200" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="I53" s="207"/>
       <c r="J53" s="345"/>
@@ -7313,15 +7313,15 @@
         <v>11</v>
       </c>
       <c r="D55" s="200" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="E55" s="207"/>
       <c r="F55" s="200" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="G55" s="207"/>
       <c r="H55" s="200" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="I55" s="207"/>
       <c r="J55" s="131"/>
@@ -7353,18 +7353,18 @@
         <v>15</v>
       </c>
       <c r="D56" s="208" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E56" s="209"/>
       <c r="F56" s="36" t="s">
         <v>64</v>
       </c>
       <c r="G56" s="347" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="H56" s="348"/>
       <c r="I56" s="187" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="J56" s="187"/>
       <c r="K56" s="116"/>
@@ -7471,7 +7471,7 @@
     <row r="59" spans="1:28" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="274"/>
       <c r="B59" s="72" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="C59" s="147"/>
       <c r="D59" s="217" t="s">
@@ -7481,7 +7481,7 @@
       <c r="F59" s="218"/>
       <c r="G59" s="219"/>
       <c r="H59" s="200" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="I59" s="207"/>
       <c r="J59" s="148"/>
@@ -7507,7 +7507,7 @@
     <row r="60" spans="1:28" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="274"/>
       <c r="B60" s="72" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="C60" s="147"/>
       <c r="D60" s="392" t="s">
@@ -7517,7 +7517,7 @@
       <c r="F60" s="393"/>
       <c r="G60" s="394"/>
       <c r="H60" s="287" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="I60" s="288"/>
       <c r="J60" s="154"/>
@@ -7549,15 +7549,15 @@
         <v>11</v>
       </c>
       <c r="D61" s="279" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E61" s="280"/>
       <c r="F61" s="296" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="G61" s="204"/>
       <c r="H61" s="296" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="I61" s="204"/>
       <c r="J61" s="11"/>
@@ -7594,11 +7594,11 @@
         <v>60</v>
       </c>
       <c r="G62" s="200" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="H62" s="207"/>
       <c r="I62" s="196" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="J62" s="197"/>
       <c r="K62" s="128"/>
@@ -7642,7 +7642,7 @@
         <v>126</v>
       </c>
       <c r="I63" s="200" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J63" s="207"/>
       <c r="K63" s="109"/>
@@ -7685,11 +7685,11 @@
         <v>71</v>
       </c>
       <c r="H64" s="192" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="I64" s="193"/>
       <c r="J64" s="192" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="K64" s="213"/>
       <c r="L64" s="2"/>
@@ -7721,7 +7721,7 @@
       </c>
       <c r="E65" s="270"/>
       <c r="F65" s="192" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G65" s="193"/>
       <c r="H65" s="200" t="s">
@@ -7755,7 +7755,7 @@
       </c>
       <c r="C66" s="207"/>
       <c r="D66" s="192" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="E66" s="193"/>
       <c r="F66" s="22" t="s">
@@ -7765,11 +7765,11 @@
         <v>89</v>
       </c>
       <c r="H66" s="192" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="I66" s="193"/>
       <c r="J66" s="252" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="K66" s="253"/>
       <c r="L66" s="2"/>
@@ -7807,11 +7807,11 @@
       </c>
       <c r="G67" s="207"/>
       <c r="H67" s="397" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="I67" s="398"/>
       <c r="J67" s="297" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K67" s="298"/>
       <c r="L67" s="2"/>
@@ -7839,7 +7839,7 @@
       </c>
       <c r="C68" s="207"/>
       <c r="D68" s="279" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="E68" s="280"/>
       <c r="F68" s="22" t="s">
@@ -7853,7 +7853,7 @@
       </c>
       <c r="I68" s="193"/>
       <c r="J68" s="200" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="K68" s="272"/>
       <c r="L68" s="2"/>
@@ -7881,7 +7881,7 @@
       </c>
       <c r="C69" s="207"/>
       <c r="D69" s="192" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="E69" s="193"/>
       <c r="F69" s="303" t="s">
@@ -7925,11 +7925,11 @@
       </c>
       <c r="E70" s="207"/>
       <c r="F70" s="200" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="G70" s="207"/>
       <c r="H70" s="399" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="I70" s="400"/>
       <c r="J70" s="257"/>
@@ -7967,7 +7967,7 @@
       </c>
       <c r="G71" s="207"/>
       <c r="H71" s="279" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I71" s="280"/>
       <c r="J71" s="246"/>
@@ -7999,15 +7999,15 @@
         <v>31</v>
       </c>
       <c r="D72" s="200" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="E72" s="207"/>
       <c r="F72" s="200" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="G72" s="207"/>
       <c r="H72" s="200" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I72" s="207"/>
       <c r="J72" s="46"/>
@@ -8045,7 +8045,7 @@
         <v>83</v>
       </c>
       <c r="F73" s="187" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="G73" s="242"/>
       <c r="H73" s="100" t="s">
@@ -8199,7 +8199,7 @@
     <row r="77" spans="1:28" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="266"/>
       <c r="B77" s="37" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="C77" s="69" t="s">
         <v>55</v>
@@ -8247,12 +8247,12 @@
       </c>
       <c r="E78" s="224"/>
       <c r="F78" s="281" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="G78" s="228"/>
       <c r="H78" s="255"/>
       <c r="I78" s="243" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="J78" s="244"/>
       <c r="K78" s="118"/>
@@ -8281,7 +8281,7 @@
       </c>
       <c r="C79" s="238"/>
       <c r="D79" s="232" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="E79" s="233"/>
       <c r="F79" s="200" t="s">
@@ -8290,7 +8290,7 @@
       <c r="G79" s="192"/>
       <c r="H79" s="255"/>
       <c r="I79" s="234" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="J79" s="234"/>
       <c r="K79" s="109"/>
@@ -8319,7 +8319,7 @@
       </c>
       <c r="C80" s="239"/>
       <c r="D80" s="232" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="E80" s="233"/>
       <c r="F80" s="42" t="s">
@@ -8330,7 +8330,7 @@
       </c>
       <c r="H80" s="255"/>
       <c r="I80" s="222" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J80" s="223"/>
       <c r="K80" s="109"/>
@@ -8361,7 +8361,7 @@
         <v>15</v>
       </c>
       <c r="D81" s="282" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E81" s="283"/>
       <c r="F81" s="192" t="s">
@@ -8399,7 +8399,7 @@
       </c>
       <c r="C82" s="238"/>
       <c r="D82" s="225" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="E82" s="226"/>
       <c r="F82" s="284" t="s">
@@ -8408,7 +8408,7 @@
       <c r="G82" s="221"/>
       <c r="H82" s="255"/>
       <c r="I82" s="222" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="J82" s="223"/>
       <c r="K82" s="109"/>
@@ -8441,12 +8441,12 @@
       </c>
       <c r="E83" s="221"/>
       <c r="F83" s="224" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="G83" s="230"/>
       <c r="H83" s="255"/>
       <c r="I83" s="222" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="J83" s="223"/>
       <c r="K83" s="107"/>
@@ -8486,7 +8486,7 @@
       <c r="G84" s="230"/>
       <c r="H84" s="255"/>
       <c r="I84" s="222" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="J84" s="223"/>
       <c r="K84" s="109"/>
@@ -8515,18 +8515,18 @@
       </c>
       <c r="C85" s="238"/>
       <c r="D85" s="185" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="E85" s="186" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="F85" s="235" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="G85" s="223"/>
       <c r="H85" s="255"/>
       <c r="I85" s="227" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="J85" s="228"/>
       <c r="K85" s="109"/>
@@ -8555,7 +8555,7 @@
       </c>
       <c r="C86" s="238"/>
       <c r="D86" s="227" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="E86" s="236"/>
       <c r="F86" s="263" t="s">
@@ -8593,14 +8593,14 @@
       </c>
       <c r="C87" s="238"/>
       <c r="D87" s="191" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E87" s="277"/>
       <c r="F87" s="235"/>
       <c r="G87" s="223"/>
       <c r="H87" s="255"/>
       <c r="I87" s="191" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="J87" s="223"/>
       <c r="K87" s="109"/>
@@ -8661,16 +8661,16 @@
       </c>
       <c r="C89" s="239"/>
       <c r="D89" s="191" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="E89" s="277"/>
       <c r="F89" s="235" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="G89" s="223"/>
       <c r="H89" s="255"/>
       <c r="I89" s="220" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J89" s="221"/>
       <c r="K89" s="109"/>
@@ -8701,16 +8701,16 @@
         <v>11</v>
       </c>
       <c r="D90" s="267" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="E90" s="268"/>
       <c r="F90" s="200" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="G90" s="353"/>
       <c r="H90" s="255"/>
       <c r="I90" s="245" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="J90" s="223"/>
       <c r="K90" s="109"/>
@@ -8741,16 +8741,16 @@
         <v>15</v>
       </c>
       <c r="D91" s="341" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E91" s="342"/>
       <c r="F91" s="187" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="G91" s="188"/>
       <c r="H91" s="256"/>
       <c r="I91" s="240" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="J91" s="241"/>
       <c r="K91" s="110"/>
@@ -36535,9 +36535,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36586,7 +36586,7 @@
       <c r="C3" s="123"/>
       <c r="D3" s="11"/>
       <c r="E3" s="10" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="F3" s="144"/>
     </row>
@@ -36597,10 +36597,10 @@
       </c>
       <c r="C4" s="123"/>
       <c r="D4" s="10" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="F4" s="169"/>
     </row>
@@ -36614,10 +36614,10 @@
         <v>146</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F5" s="144" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="66" x14ac:dyDescent="0.25">
@@ -36627,13 +36627,13 @@
       </c>
       <c r="C6" s="417"/>
       <c r="D6" s="10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="F6" s="144" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="66" x14ac:dyDescent="0.25">
@@ -36643,10 +36643,10 @@
       </c>
       <c r="C7" s="418"/>
       <c r="D7" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F7" s="168"/>
     </row>
@@ -36657,13 +36657,13 @@
       </c>
       <c r="C8" s="418"/>
       <c r="D8" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F8" s="179" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="66" x14ac:dyDescent="0.25">
@@ -36673,42 +36673,42 @@
       </c>
       <c r="C9" s="418"/>
       <c r="D9" s="10" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F9" s="179" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="66" x14ac:dyDescent="0.25">
       <c r="A10" s="415"/>
       <c r="B10" s="165" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C10" s="418"/>
       <c r="D10" s="10" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F10" s="144" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="415"/>
       <c r="B11" s="165" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="C11" s="151"/>
       <c r="E11" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="F11" s="144" t="s">
         <v>177</v>
-      </c>
-      <c r="F11" s="144" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="66" x14ac:dyDescent="0.25">
@@ -36719,10 +36719,10 @@
       <c r="C12" s="151"/>
       <c r="D12" s="11"/>
       <c r="E12" s="10" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F12" s="179" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="66" x14ac:dyDescent="0.25">
@@ -36733,10 +36733,10 @@
       <c r="C13" s="152"/>
       <c r="D13" s="166"/>
       <c r="E13" s="10" t="s">
-        <v>195</v>
+        <v>325</v>
       </c>
       <c r="F13" s="144" t="s">
-        <v>196</v>
+        <v>326</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -36747,7 +36747,7 @@
       <c r="C14" s="180"/>
       <c r="D14" s="173"/>
       <c r="E14" s="173" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F14" s="174"/>
     </row>
@@ -36787,7 +36787,7 @@
       <c r="C17" s="123"/>
       <c r="D17" s="133"/>
       <c r="E17" s="10" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="F17" s="167"/>
     </row>
@@ -36799,7 +36799,7 @@
       <c r="C18" s="418"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F18" s="169"/>
     </row>
@@ -36810,13 +36810,13 @@
       </c>
       <c r="C19" s="418"/>
       <c r="D19" s="10" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F19" s="144" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="66" x14ac:dyDescent="0.25">
@@ -36826,13 +36826,13 @@
       </c>
       <c r="C20" s="418"/>
       <c r="D20" s="10" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F20" s="144" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="66" x14ac:dyDescent="0.25">
@@ -36842,13 +36842,13 @@
       </c>
       <c r="C21" s="418"/>
       <c r="D21" s="10" t="s">
-        <v>149</v>
+        <v>329</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>197</v>
+        <v>327</v>
       </c>
       <c r="F21" s="144" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="66" x14ac:dyDescent="0.25">
@@ -36858,13 +36858,13 @@
       </c>
       <c r="C22" s="123"/>
       <c r="D22" s="10" t="s">
-        <v>159</v>
+        <v>328</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F22" s="144" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="78" x14ac:dyDescent="0.25">
@@ -36874,13 +36874,13 @@
       </c>
       <c r="C23" s="123"/>
       <c r="D23" s="153" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E23" s="153" t="s">
+        <v>184</v>
+      </c>
+      <c r="F23" s="144" t="s">
         <v>186</v>
-      </c>
-      <c r="F23" s="144" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="78" x14ac:dyDescent="0.25">
@@ -36890,27 +36890,27 @@
       </c>
       <c r="C24" s="176"/>
       <c r="D24" s="177" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="E24" s="177" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F24" s="178"/>
     </row>
     <row r="25" spans="1:6" ht="78.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="170"/>
       <c r="B25" s="171" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C25" s="171"/>
       <c r="D25" s="172" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="E25" s="173" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="F25" s="174" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>

</xml_diff>